<commit_message>
Se agrega validación de fecha para Ecuaquimica en SellOut.exe
</commit_message>
<xml_diff>
--- a/output/SellOut/Base clientes.xlsx
+++ b/output/SellOut/Base clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad2196898358a5cd/Documentos/SellOut ConAgro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_4A73B0EAC3FF00B02A8C7BF8D40FB3D6B6066E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E88AAFA-2DF8-4940-B9BD-8D2D4A96BBC7}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_4A73B0EAC3FF00B02A8C7BF8D40FB3D6B6066E62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45E4D1FD-410C-4866-856B-35DB1D295115}"/>
   <bookViews>
     <workbookView xWindow="26280" yWindow="1170" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +515,7 @@
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>61610107</v>
+        <v>61610097</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>

</xml_diff>